<commit_message>
New CR and IR top 5 calcs and plots; and other random updates from before I went to Dallas 9/4/23
</commit_message>
<xml_diff>
--- a/data7_24/Abundance/AB_allEvents.xlsx
+++ b/data7_24/Abundance/AB_allEvents.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/allisonadams/Documents/Thesis/Microplankton/R Work/MicroplanktonAnalysis/data/Abundance/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/allisonadams/My files/Thesis/Microplankton/MicroplanktonAnalysis/data7_24/Abundance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF54AE24-9007-E140-A7A9-2D33C70B05E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E046619A-1972-8540-8503-B54F5EC8CAA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3380" yWindow="500" windowWidth="16240" windowHeight="11680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,9 +38,6 @@
     <t>taxaGroup</t>
   </si>
   <si>
-    <t>TotalCpmI</t>
-  </si>
-  <si>
     <t>CenDiaLg</t>
   </si>
   <si>
@@ -113,6 +110,9 @@
       </rPr>
       <t>-1</t>
     </r>
+  </si>
+  <si>
+    <t>MeanCpmI</t>
   </si>
 </sst>
 </file>
@@ -493,7 +493,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -506,194 +506,194 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="2">
         <v>864.88239659463795</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="2">
         <v>267.16502149248578</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="2">
         <v>225.93189495616161</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" s="2">
         <v>76.439971480685301</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="2">
         <v>44.705886365436378</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="2">
         <v>38.400210798416907</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="2">
         <v>34.035910561618543</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" s="2">
         <v>19.89372785380581</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" s="2">
         <v>11.04875702645638</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="2">
         <v>5.2006683867912153</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" s="2">
         <v>4.2228856623463944</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B13" s="2">
         <v>3.8641758060867528</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" s="2">
         <v>2.3288785544645361</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B15" s="2">
         <v>2.012042627119444</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B16" s="2">
         <v>1.555989017655494</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B17" s="2">
         <v>0.86423889110197161</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B18" s="2">
         <v>4.3844375761884387E-2</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>